<commit_message>
Agrego la mejor version del modelo actual
</commit_message>
<xml_diff>
--- a/docs/Planning_Gantt.xlsx
+++ b/docs/Planning_Gantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="306" documentId="8_{5AF800A2-D3CD-42C0-84D0-DB173922EFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{777234D2-D97E-4279-B7FD-3CEA85D1495C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177B3298-C825-47CC-8CC2-F4D0F59CE430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1314,7 +1314,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="6" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1440,7 +1440,7 @@
     <xf numFmtId="168" fontId="40" fillId="45" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="40" fillId="6" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="168" fontId="40" fillId="6" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1452,7 +1452,7 @@
     <xf numFmtId="167" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
@@ -1802,10 +1802,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2075,8 +2071,8 @@
   <dimension ref="A1:BL44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB40" sqref="AB40"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2142,11 +2138,11 @@
       </c>
       <c r="D4" s="87"/>
       <c r="E4" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I4" s="82">
         <f>I5</f>
-        <v>44977</v>
+        <v>45026</v>
       </c>
       <c r="J4" s="83"/>
       <c r="K4" s="83"/>
@@ -2156,7 +2152,7 @@
       <c r="O4" s="84"/>
       <c r="P4" s="82">
         <f>P5</f>
-        <v>44984</v>
+        <v>45033</v>
       </c>
       <c r="Q4" s="83"/>
       <c r="R4" s="83"/>
@@ -2166,7 +2162,7 @@
       <c r="V4" s="84"/>
       <c r="W4" s="82">
         <f>W5</f>
-        <v>44991</v>
+        <v>45040</v>
       </c>
       <c r="X4" s="83"/>
       <c r="Y4" s="83"/>
@@ -2176,7 +2172,7 @@
       <c r="AC4" s="84"/>
       <c r="AD4" s="82">
         <f>AD5</f>
-        <v>44998</v>
+        <v>45047</v>
       </c>
       <c r="AE4" s="83"/>
       <c r="AF4" s="83"/>
@@ -2186,7 +2182,7 @@
       <c r="AJ4" s="84"/>
       <c r="AK4" s="82">
         <f>AK5</f>
-        <v>45005</v>
+        <v>45054</v>
       </c>
       <c r="AL4" s="83"/>
       <c r="AM4" s="83"/>
@@ -2196,7 +2192,7 @@
       <c r="AQ4" s="84"/>
       <c r="AR4" s="82">
         <f>AR5</f>
-        <v>45012</v>
+        <v>45061</v>
       </c>
       <c r="AS4" s="83"/>
       <c r="AT4" s="83"/>
@@ -2206,7 +2202,7 @@
       <c r="AX4" s="84"/>
       <c r="AY4" s="82">
         <f>AY5</f>
-        <v>45019</v>
+        <v>45068</v>
       </c>
       <c r="AZ4" s="83"/>
       <c r="BA4" s="83"/>
@@ -2216,7 +2212,7 @@
       <c r="BE4" s="84"/>
       <c r="BF4" s="82">
         <f>BF5</f>
-        <v>45026</v>
+        <v>45075</v>
       </c>
       <c r="BG4" s="83"/>
       <c r="BH4" s="83"/>
@@ -2237,227 +2233,227 @@
       <c r="G5" s="35"/>
       <c r="I5" s="40">
         <f>Inicio_del_proyecto-WEEKDAY(Inicio_del_proyecto,1)+2+7*(Semana_para_mostrar-1)</f>
-        <v>44977</v>
+        <v>45026</v>
       </c>
       <c r="J5" s="41">
         <f>I5+1</f>
-        <v>44978</v>
+        <v>45027</v>
       </c>
       <c r="K5" s="41">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>44979</v>
+        <v>45028</v>
       </c>
       <c r="L5" s="41">
         <f t="shared" si="0"/>
-        <v>44980</v>
+        <v>45029</v>
       </c>
       <c r="M5" s="41">
         <f t="shared" si="0"/>
-        <v>44981</v>
+        <v>45030</v>
       </c>
       <c r="N5" s="41">
         <f t="shared" si="0"/>
-        <v>44982</v>
+        <v>45031</v>
       </c>
       <c r="O5" s="42">
         <f t="shared" si="0"/>
-        <v>44983</v>
+        <v>45032</v>
       </c>
       <c r="P5" s="40">
         <f>O5+1</f>
-        <v>44984</v>
+        <v>45033</v>
       </c>
       <c r="Q5" s="41">
         <f>P5+1</f>
-        <v>44985</v>
+        <v>45034</v>
       </c>
       <c r="R5" s="41">
         <f t="shared" si="0"/>
-        <v>44986</v>
+        <v>45035</v>
       </c>
       <c r="S5" s="41">
         <f t="shared" si="0"/>
-        <v>44987</v>
+        <v>45036</v>
       </c>
       <c r="T5" s="41">
         <f t="shared" si="0"/>
-        <v>44988</v>
+        <v>45037</v>
       </c>
       <c r="U5" s="41">
         <f t="shared" si="0"/>
-        <v>44989</v>
+        <v>45038</v>
       </c>
       <c r="V5" s="42">
         <f t="shared" si="0"/>
-        <v>44990</v>
+        <v>45039</v>
       </c>
       <c r="W5" s="40">
         <f>V5+1</f>
-        <v>44991</v>
+        <v>45040</v>
       </c>
       <c r="X5" s="41">
         <f>W5+1</f>
-        <v>44992</v>
+        <v>45041</v>
       </c>
       <c r="Y5" s="41">
         <f t="shared" si="0"/>
-        <v>44993</v>
+        <v>45042</v>
       </c>
       <c r="Z5" s="41">
         <f t="shared" si="0"/>
-        <v>44994</v>
+        <v>45043</v>
       </c>
       <c r="AA5" s="41">
         <f t="shared" si="0"/>
-        <v>44995</v>
+        <v>45044</v>
       </c>
       <c r="AB5" s="41">
         <f t="shared" si="0"/>
-        <v>44996</v>
+        <v>45045</v>
       </c>
       <c r="AC5" s="42">
         <f t="shared" si="0"/>
-        <v>44997</v>
+        <v>45046</v>
       </c>
       <c r="AD5" s="40">
         <f>AC5+1</f>
-        <v>44998</v>
+        <v>45047</v>
       </c>
       <c r="AE5" s="41">
         <f>AD5+1</f>
-        <v>44999</v>
+        <v>45048</v>
       </c>
       <c r="AF5" s="41">
         <f t="shared" si="0"/>
-        <v>45000</v>
+        <v>45049</v>
       </c>
       <c r="AG5" s="41">
         <f t="shared" si="0"/>
-        <v>45001</v>
+        <v>45050</v>
       </c>
       <c r="AH5" s="41">
         <f t="shared" si="0"/>
-        <v>45002</v>
+        <v>45051</v>
       </c>
       <c r="AI5" s="41">
         <f t="shared" si="0"/>
-        <v>45003</v>
+        <v>45052</v>
       </c>
       <c r="AJ5" s="42">
         <f t="shared" si="0"/>
-        <v>45004</v>
+        <v>45053</v>
       </c>
       <c r="AK5" s="40">
         <f>AJ5+1</f>
-        <v>45005</v>
+        <v>45054</v>
       </c>
       <c r="AL5" s="41">
         <f>AK5+1</f>
-        <v>45006</v>
+        <v>45055</v>
       </c>
       <c r="AM5" s="41">
         <f t="shared" si="0"/>
-        <v>45007</v>
+        <v>45056</v>
       </c>
       <c r="AN5" s="41">
         <f t="shared" si="0"/>
-        <v>45008</v>
+        <v>45057</v>
       </c>
       <c r="AO5" s="41">
         <f t="shared" si="0"/>
-        <v>45009</v>
+        <v>45058</v>
       </c>
       <c r="AP5" s="41">
         <f t="shared" si="0"/>
-        <v>45010</v>
+        <v>45059</v>
       </c>
       <c r="AQ5" s="42">
         <f t="shared" si="0"/>
-        <v>45011</v>
+        <v>45060</v>
       </c>
       <c r="AR5" s="40">
         <f>AQ5+1</f>
-        <v>45012</v>
+        <v>45061</v>
       </c>
       <c r="AS5" s="41">
         <f>AR5+1</f>
-        <v>45013</v>
+        <v>45062</v>
       </c>
       <c r="AT5" s="41">
         <f t="shared" si="0"/>
-        <v>45014</v>
+        <v>45063</v>
       </c>
       <c r="AU5" s="41">
         <f t="shared" si="0"/>
-        <v>45015</v>
+        <v>45064</v>
       </c>
       <c r="AV5" s="41">
         <f t="shared" si="0"/>
-        <v>45016</v>
+        <v>45065</v>
       </c>
       <c r="AW5" s="41">
         <f t="shared" si="0"/>
-        <v>45017</v>
+        <v>45066</v>
       </c>
       <c r="AX5" s="42">
         <f t="shared" si="0"/>
-        <v>45018</v>
+        <v>45067</v>
       </c>
       <c r="AY5" s="40">
         <f>AX5+1</f>
-        <v>45019</v>
+        <v>45068</v>
       </c>
       <c r="AZ5" s="41">
         <f>AY5+1</f>
-        <v>45020</v>
+        <v>45069</v>
       </c>
       <c r="BA5" s="41">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45021</v>
+        <v>45070</v>
       </c>
       <c r="BB5" s="41">
         <f t="shared" si="1"/>
-        <v>45022</v>
+        <v>45071</v>
       </c>
       <c r="BC5" s="41">
         <f t="shared" si="1"/>
-        <v>45023</v>
+        <v>45072</v>
       </c>
       <c r="BD5" s="41">
         <f t="shared" si="1"/>
-        <v>45024</v>
+        <v>45073</v>
       </c>
       <c r="BE5" s="42">
         <f t="shared" si="1"/>
-        <v>45025</v>
+        <v>45074</v>
       </c>
       <c r="BF5" s="40">
         <f>BE5+1</f>
-        <v>45026</v>
+        <v>45075</v>
       </c>
       <c r="BG5" s="41">
         <f>BF5+1</f>
-        <v>45027</v>
+        <v>45076</v>
       </c>
       <c r="BH5" s="41">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>45028</v>
+        <v>45077</v>
       </c>
       <c r="BI5" s="41">
         <f t="shared" si="2"/>
-        <v>45029</v>
+        <v>45078</v>
       </c>
       <c r="BJ5" s="41">
         <f t="shared" si="2"/>
-        <v>45030</v>
+        <v>45079</v>
       </c>
       <c r="BK5" s="41">
         <f t="shared" si="2"/>
-        <v>45031</v>
+        <v>45080</v>
       </c>
       <c r="BL5" s="42">
         <f t="shared" si="2"/>
-        <v>45032</v>
+        <v>45081</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3094,7 +3090,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="61">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E12" s="43">
         <f>DATE(2023,3,1)</f>
@@ -3175,7 +3171,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="43">
         <f>DATE(2023,3,1)</f>
@@ -3258,7 +3254,7 @@
         <v>49</v>
       </c>
       <c r="D14" s="61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="43">
         <f>DATE(2023,3,1)</f>
@@ -3339,7 +3335,7 @@
         <v>50</v>
       </c>
       <c r="D15" s="61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="43">
         <f>F14+1</f>
@@ -3420,7 +3416,7 @@
         <v>51</v>
       </c>
       <c r="D16" s="61">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E16" s="43">
         <f>DATE(2023,3,11)</f>
@@ -3572,7 +3568,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="80">
         <v>44991</v>
@@ -3651,7 +3647,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="77">
         <f>F18</f>
@@ -3734,7 +3730,7 @@
         <v>54</v>
       </c>
       <c r="D20" s="66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="44">
         <f>E19</f>
@@ -3815,7 +3811,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="44">
         <f>F20</f>
@@ -3896,7 +3892,7 @@
         <v>56</v>
       </c>
       <c r="D22" s="66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="44">
         <f>E21+5</f>
@@ -3977,7 +3973,7 @@
         <v>61</v>
       </c>
       <c r="D23" s="66">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E23" s="44">
         <f>F22</f>
@@ -4058,7 +4054,7 @@
         <v>62</v>
       </c>
       <c r="D24" s="66">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E24" s="44">
         <f>F23</f>
@@ -4139,7 +4135,7 @@
         <v>64</v>
       </c>
       <c r="D25" s="66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="79">
         <f>DATE(2023,4,17)</f>
@@ -5906,35 +5902,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6222,27 +6189,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6261,4 +6237,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>